<commit_message>
Wording changes from PM&C.
</commit_message>
<xml_diff>
--- a/dashboard_loader/health_agedcare_uploader/health_agedcare.xlsx
+++ b/dashboard_loader/health_agedcare_uploader/health_agedcare.xlsx
@@ -86,7 +86,25 @@
     <t xml:space="preserve">Desc Body</t>
   </si>
   <si>
-    <t xml:space="preserve">The Commonwealth Government has set a target of 125 places per 1000 people aged 70 years and over by 2020–21 (DSS, 2013). </t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">The Commonwealth Government has set a target of 125 places per 1000 people aged 70 years and over by 2021-22. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">The Commonwealth funds and regulates residential and home-based aged care services.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">The growth in the rate of aged care places has stalled in recent years. After increasing in 2010 and 2011, rates of aged care places have remained around 108 places per 1000 people from 2012 to 2016.</t>
@@ -130,7 +148,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -239,6 +257,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -434,7 +458,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -539,7 +563,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B8:B12 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1168,7 +1192,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B8:B12"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1210,7 +1234,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="37.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>

</xml_diff>